<commit_message>
[Jimmy] modificacion de las pantallas de pagos a proveedores y empleados
</commit_message>
<xml_diff>
--- a/src/assets/anexos/Anexo_pago_a_empleados.xlsx
+++ b/src/assets/anexos/Anexo_pago_a_empleados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Documents/Edgar/coop-ifi-front-personas/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF3F14B-180E-8F49-8840-2F0B301B9AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C30AD91-1673-FA46-BBCA-B6A791E5B524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26880" yWindow="3000" windowWidth="18900" windowHeight="12520" xr2:uid="{7C2F3D3F-1238-4BD7-AFBB-6E6A76A02282}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19320" xr2:uid="{7C2F3D3F-1238-4BD7-AFBB-6E6A76A02282}"/>
   </bookViews>
   <sheets>
     <sheet name="Pagos" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Fecha</t>
   </si>
@@ -80,13 +80,22 @@
   </si>
   <si>
     <t>Yar</t>
+  </si>
+  <si>
+    <t>Número de cuenta bancaria del empleado</t>
+  </si>
+  <si>
+    <t>Banco destino</t>
+  </si>
+  <si>
+    <t>Banco pichincha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +111,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -111,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,23 +136,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -453,57 +488,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCC3E15-B35D-4098-8E90-1863ADD9BB1D}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="10.83203125" style="4"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="2"/>
     <col min="9" max="9" width="10.83203125" style="2"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.83203125" customWidth="1"/>
+    <col min="11" max="11" width="38.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>45109</v>
       </c>
       <c r="B2" t="s">
@@ -532,6 +575,12 @@
       </c>
       <c r="J2" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2206282211</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Jimmy] correcion de enviar informacion del propietario de la firma y el formato de documento excel
</commit_message>
<xml_diff>
--- a/src/assets/anexos/Anexo_pago_a_empleados.xlsx
+++ b/src/assets/anexos/Anexo_pago_a_empleados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Documents/Edgar/coop-ifi-front-personas/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C30AD91-1673-FA46-BBCA-B6A791E5B524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC64A3-BD65-D64B-8D25-C9B0617C21F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19320" xr2:uid="{7C2F3D3F-1238-4BD7-AFBB-6E6A76A02282}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19160" xr2:uid="{7C2F3D3F-1238-4BD7-AFBB-6E6A76A02282}"/>
   </bookViews>
   <sheets>
     <sheet name="Pagos" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,9 +168,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -491,18 +488,18 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="4"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="10.83203125" style="2"/>
-    <col min="10" max="10" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.83203125" style="2"/>
+    <col min="10" max="10" width="27.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="38.6640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="23.83203125" style="2" customWidth="1"/>
   </cols>
@@ -511,31 +508,31 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -549,13 +546,13 @@
       <c r="A2" s="4">
         <v>45109</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>2023</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>400</v>
       </c>
       <c r="E2" s="2">
@@ -564,10 +561,10 @@
       <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="2" t="s">

</xml_diff>